<commit_message>
Updated BOM to include product links
</commit_message>
<xml_diff>
--- a/KEYBOARD_BOM.xlsx
+++ b/KEYBOARD_BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>Product name</t>
   </si>
@@ -34,36 +34,56 @@
     <t>Notes</t>
   </si>
   <si>
+    <t>LINKS</t>
+  </si>
+  <si>
     <t>OLED Module 0.91" 128x32</t>
   </si>
   <si>
     <t>OLED display module</t>
   </si>
   <si>
+    <t>https://grobotronics.com/oled-module-0.91-128x32-i2c-white.html</t>
+  </si>
+  <si>
     <t>Rotary Encoder 12mm 24P/R with Switch</t>
   </si>
   <si>
     <t>Rotary Encoder with Switch</t>
   </si>
   <si>
+    <t xml:space="preserve">https://grobotronics.com/rotary-encoder-12mm-24p-r-with-switch.html
+</t>
+  </si>
+  <si>
     <t>74AHCT125</t>
   </si>
   <si>
     <t>Quad Level-Shifter</t>
   </si>
   <si>
+    <t>https://grobotronics.com/74ahct125-quad-level-shifter.html</t>
+  </si>
+  <si>
     <t>SK6812</t>
   </si>
   <si>
     <t>LED SMD 5050 RGB Programmable</t>
   </si>
   <si>
+    <t xml:space="preserve">https://grobotronics.com/led-8mm-rgb-programmable-ws2812-clone.html
+</t>
+  </si>
+  <si>
     <t>74HCT595D</t>
   </si>
   <si>
     <t>Shift Register 8-Bit SMD</t>
   </si>
   <si>
+    <t>https://grobotronics.com/shift-register-8-bit-smd-74hct595d.html</t>
+  </si>
+  <si>
     <t>Capacitor 1000uF</t>
   </si>
   <si>
@@ -73,18 +93,28 @@
     <t>with 2.20 shipping from grobotronics for last 6 products</t>
   </si>
   <si>
+    <t xml:space="preserve">https://grobotronics.com/electrolytic-capacitor-16v-1000ufoem.html
+</t>
+  </si>
+  <si>
     <t>Πυκνωτής 100nf</t>
   </si>
   <si>
     <t>Πυκνωτής Κεραμικός 104(100nf)</t>
   </si>
   <si>
+    <t>https://nettop.gr/index.php/hlektronika/capacitors/ceramic-capacitor/pyknotis-keramikos-104-100nf.html</t>
+  </si>
+  <si>
     <t>Raspberry Pi Pico</t>
   </si>
   <si>
     <t>Raspberry Pi Pico without Headers</t>
   </si>
   <si>
+    <t>https://nettop.gr/index.php/raspberry-pi/pico/raspberry-pi-pico.html?src=raspberrypi</t>
+  </si>
+  <si>
     <t>1N4148</t>
   </si>
   <si>
@@ -94,6 +124,9 @@
     <t>with 2.30 shipping from nettop for last 3 products</t>
   </si>
   <si>
+    <t>https://nettop.gr/index.php/hlektronika/diode/diode-1n4148-small-signal-fast-switching-diode.html</t>
+  </si>
+  <si>
     <t>Keychron K Pro Switches</t>
   </si>
   <si>
@@ -103,15 +136,24 @@
     <t>in-store pickup</t>
   </si>
   <si>
+    <t>https://www.public.gr/product/gaming/pc-gaming/pc-gaming-accessories/diafora-pc-gaming-accessories/keychron-k-pro-switches-pliktrologiou-110-pack/2090270</t>
+  </si>
+  <si>
     <t>Glorious Stabilizers V2</t>
   </si>
   <si>
+    <t>https://shopflix.gr/p/SF-12868640/stabilizers-glorious-v2-gata1723-12843162</t>
+  </si>
+  <si>
     <t>Mountain Dolomite A Backlit Keycap Set</t>
   </si>
   <si>
     <t>with 5 shipping from shopflix for last 2 products</t>
   </si>
   <si>
+    <t>https://www.skroutz.gr/s/57409660/Mountain-Dolomite-A-Backlit-Keycap-Set.html</t>
+  </si>
+  <si>
     <t>PCB</t>
   </si>
   <si>
@@ -119,13 +161,19 @@
   </si>
   <si>
     <t>with cheapest shipping</t>
+  </si>
+  <si>
+    <t>https://shopflix.gr/p/SF-200097568/mountain-dolomite-a-backlit-keycap-set</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -136,6 +184,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,11 +208,17 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
@@ -410,13 +472,16 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1">
         <v>1.0</v>
@@ -430,13 +495,16 @@
       <c r="F2" s="1">
         <v>6.8</v>
       </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>2.0</v>
@@ -451,13 +519,16 @@
         <f>6.8+2.4</f>
         <v>9.2</v>
       </c>
+      <c r="H3" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1">
         <v>1.0</v>
@@ -471,13 +542,16 @@
       <c r="F4" s="1">
         <v>9.7</v>
       </c>
+      <c r="H4" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1">
         <v>10.0</v>
@@ -491,13 +565,16 @@
       <c r="F5" s="1">
         <v>12.7</v>
       </c>
+      <c r="H5" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1">
         <v>2.0</v>
@@ -511,13 +588,16 @@
       <c r="F6" s="1">
         <v>14.3</v>
       </c>
+      <c r="H6" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1">
         <v>1.0</v>
@@ -532,15 +612,18 @@
         <v>16.7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1">
         <v>2.0</v>
@@ -554,13 +637,16 @@
       <c r="F8" s="1">
         <v>16.8</v>
       </c>
+      <c r="H8" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1">
         <v>1.0</v>
@@ -571,17 +657,20 @@
       <c r="E9" s="1">
         <v>4.2</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="4">
         <f>16.8+4.2</f>
         <v>21</v>
       </c>
+      <c r="H9" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1">
         <v>110.0</v>
@@ -592,20 +681,23 @@
       <c r="E10" s="1">
         <v>4.4</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="4">
         <f>21+4.4+2.3</f>
         <v>27.7</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1">
         <v>1.0</v>
@@ -616,20 +708,23 @@
       <c r="E11" s="1">
         <v>17.48</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="4">
         <f>17.48+27.7</f>
         <v>45.18</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1">
         <v>1.0</v>
@@ -640,41 +735,47 @@
       <c r="E12" s="1">
         <v>4.99</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="4">
         <f>45.18+4.99</f>
         <v>50.17</v>
       </c>
+      <c r="H12" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1">
         <v>1.0</v>
       </c>
       <c r="D13" s="1">
-        <v>5.22</v>
+        <v>5.25</v>
       </c>
       <c r="E13" s="1">
-        <v>5.22</v>
-      </c>
-      <c r="F13" s="2">
-        <f>5.22+F12+5</f>
-        <v>60.39</v>
+        <v>5.25</v>
+      </c>
+      <c r="F13" s="1">
+        <f>5.25+F12+5</f>
+        <v>60.42</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1">
         <v>42.33</v>
@@ -685,15 +786,39 @@
       <c r="E14" s="1">
         <v>42.33</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="4">
         <f>F13+42.33</f>
-        <v>102.72</v>
+        <v>102.75</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>35</v>
+        <v>48</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="H15" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="H2"/>
+    <hyperlink r:id="rId2" ref="H3"/>
+    <hyperlink r:id="rId3" ref="H4"/>
+    <hyperlink r:id="rId4" ref="H5"/>
+    <hyperlink r:id="rId5" ref="H6"/>
+    <hyperlink r:id="rId6" ref="H7"/>
+    <hyperlink r:id="rId7" ref="H8"/>
+    <hyperlink r:id="rId8" ref="H9"/>
+    <hyperlink r:id="rId9" ref="H10"/>
+    <hyperlink r:id="rId10" ref="H11"/>
+    <hyperlink r:id="rId11" ref="H12"/>
+    <hyperlink r:id="rId12" ref="H13"/>
+    <hyperlink r:id="rId13" ref="H14"/>
+    <hyperlink r:id="rId14" ref="H15"/>
+  </hyperlinks>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>